<commit_message>
Update API Security Testing Excel files
- Updated multiple API Security Testing Excel files to incorporate the latest data and insights on API security concerns, effectiveness, and lifecycle benefits.
</commit_message>
<xml_diff>
--- a/data/Section 3/3.5 API Security Testing/18 API Security Testing- Concern.xlsx
+++ b/data/Section 3/3.5 API Security Testing/18 API Security Testing- Concern.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Section 3/3.5 API Security Testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Survey Report Agent/surveyreport/data/Section 3/3.5 API Security Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{9A0B95CB-C758-44CB-AF7B-A52E1A1AA7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEAFB3C9-8777-41EF-BC5F-AC84356E5EC5}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{9A0B95CB-C758-44CB-AF7B-A52E1A1AA7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C678F96-9CC8-4EFD-8237-5C06F2F26A3A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9D2E9AC6-8497-4553-A052-F400E787F5AC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$G$1001</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,30 +39,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4015" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4017" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -124,28 +102,34 @@
     <t>Code-based discovery (e.g., static/dynamic code analysis)</t>
   </si>
   <si>
-    <t xml:space="preserve">5 - Extremely Concerning </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 - Highly Concerning </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 - Slightly Concerning </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 - Moderately Concerning </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 - Minimal Concern </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0 - No Concern </t>
-  </si>
-  <si>
     <t>Crawler-based discovery (e.g., scanning APIs)</t>
   </si>
   <si>
     <t>Traffic-based discovery (e.g., monitoring API traffic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No Concern </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Minimal Concern </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slightly Concerning </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Moderately Concerning </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Highly Concerning </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Extremely Concerning </t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -269,6 +253,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{31E36893-1ACD-44B8-B600-A26154BFB931}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{31E36893-1ACD-44B8-B600-A26154BFB931}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{7E3A85D6-C31E-4404-8DBF-2F454FFAB634}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{DDCAE3A5-F98F-42A2-B114-5D23DCD3D37C}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -624,10 +619,10 @@
         <v>19</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -29638,126 +29633,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C4F6D3F-9092-4C2D-90DA-206924F74C2A}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="11.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" cm="1">
-        <f t="array" ref="A1:A6">_xlfn._xlws.SORT(_xlfn.UNIQUE(Sheet1!G2:G1001))</f>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>0</v>
       </c>
-      <c r="B1" cm="1">
-        <f t="array" ref="B1:B6">_xlfn._xlws.SORT(_xlfn.UNIQUE(Sheet1!H2:H1001))</f>
-        <v>0</v>
-      </c>
-      <c r="C1" cm="1">
-        <f t="array" ref="C1:C6">_xlfn._xlws.SORT(_xlfn.UNIQUE(Sheet1!I2:I1001))</f>
-        <v>0</v>
-      </c>
-      <c r="D1" cm="1">
-        <f t="array" ref="D1">_xlfn._xlws.SORT(_xlfn.UNIQUE(Sheet1!J2:J1001))</f>
-        <v>0</v>
-      </c>
-      <c r="E1" cm="1">
-        <f t="array" ref="E1">_xlfn._xlws.SORT(_xlfn.UNIQUE(Sheet1!K2:K1001))</f>
-        <v>0</v>
-      </c>
-      <c r="F1" cm="1">
-        <f t="array" ref="F1">_xlfn._xlws.SORT(_xlfn.UNIQUE(Sheet1!L2:L1001))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
+      <c r="B7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>